<commit_message>
Adding to naming, flours
</commit_message>
<xml_diff>
--- a/FluorophoreProps.xlsx
+++ b/FluorophoreProps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22170" windowHeight="10890"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28185" windowHeight="10875"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="66">
   <si>
     <t>Quantum Yield</t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>EYFP</t>
+  </si>
+  <si>
+    <t>mScarlet-I</t>
   </si>
 </sst>
 </file>
@@ -589,13 +592,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH35"/>
+  <dimension ref="A1:AI35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="J8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="Q10" sqref="Q10"/>
+      <selection pane="bottomRight" activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,12 +606,12 @@
     <col min="1" max="1" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -625,7 +628,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -665,38 +668,38 @@
       <c r="V5" t="s">
         <v>58</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>1</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>7</v>
       </c>
-      <c r="Z5">
+      <c r="AA5">
         <v>7</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>59</v>
       </c>
       <c r="AC5" t="s">
         <v>59</v>
       </c>
-      <c r="AD5">
-        <v>5</v>
+      <c r="AD5" t="s">
+        <v>59</v>
       </c>
       <c r="AE5">
         <v>5</v>
       </c>
       <c r="AF5">
+        <v>5</v>
+      </c>
+      <c r="AG5">
         <v>8</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AH5" t="s">
         <v>59</v>
       </c>
-      <c r="AH5">
+      <c r="AI5">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -764,43 +767,46 @@
         <v>48</v>
       </c>
       <c r="W7" t="s">
+        <v>65</v>
+      </c>
+      <c r="X7" t="s">
         <v>7</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Y7" t="s">
         <v>42</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="Z7" t="s">
         <v>49</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>43</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AB7" t="s">
         <v>50</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AC7" t="s">
         <v>51</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>52</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AE7" t="s">
         <v>8</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AF7" t="s">
         <v>9</v>
       </c>
-      <c r="AF7" t="s">
+      <c r="AG7" t="s">
         <v>54</v>
       </c>
-      <c r="AG7" t="s">
+      <c r="AH7" t="s">
         <v>55</v>
       </c>
-      <c r="AH7" t="s">
+      <c r="AI7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -868,37 +874,40 @@
         <v>0.15</v>
       </c>
       <c r="W8">
+        <v>0.54</v>
+      </c>
+      <c r="X8">
         <v>0.22</v>
       </c>
-      <c r="X8">
+      <c r="Y8">
         <v>0.4</v>
       </c>
-      <c r="Y8">
+      <c r="Z8">
         <v>0.66</v>
       </c>
-      <c r="Z8">
+      <c r="AA8">
         <v>0.19</v>
-      </c>
-      <c r="AB8">
-        <v>0.3</v>
       </c>
       <c r="AC8">
         <v>0.3</v>
       </c>
       <c r="AD8">
+        <v>0.3</v>
+      </c>
+      <c r="AE8">
         <v>0.33</v>
       </c>
-      <c r="AE8">
+      <c r="AF8">
         <v>0.36</v>
       </c>
-      <c r="AF8">
+      <c r="AG8">
         <v>0.25</v>
       </c>
-      <c r="AH8">
+      <c r="AI8">
         <v>0.12</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -917,16 +926,19 @@
         <v>30</v>
       </c>
       <c r="W9">
+        <v>36</v>
+      </c>
+      <c r="X9">
         <v>15</v>
       </c>
-      <c r="X9">
+      <c r="Y9">
         <v>20</v>
       </c>
-      <c r="Z9">
+      <c r="AA9">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -948,20 +960,23 @@
       <c r="T10">
         <v>4.0999999999999996</v>
       </c>
-      <c r="Y10">
+      <c r="W10">
+        <v>3.1</v>
+      </c>
+      <c r="Z10">
         <v>3.9</v>
       </c>
-      <c r="AA10">
+      <c r="AB10">
         <v>3.2</v>
       </c>
-      <c r="AD10">
+      <c r="AE10">
         <v>1</v>
       </c>
-      <c r="AE10">
+      <c r="AF10">
         <v>1.2</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1029,43 +1044,46 @@
         <v>150000</v>
       </c>
       <c r="W11">
+        <v>104000</v>
+      </c>
+      <c r="X11">
         <v>72000</v>
       </c>
-      <c r="X11">
+      <c r="Y11">
         <v>62500</v>
       </c>
-      <c r="Y11">
+      <c r="Z11">
         <v>92000</v>
       </c>
-      <c r="Z11">
+      <c r="AA11">
         <v>87000</v>
       </c>
-      <c r="AA11">
+      <c r="AB11">
         <v>159000</v>
       </c>
-      <c r="AB11">
+      <c r="AC11">
         <v>250000</v>
       </c>
-      <c r="AC11">
+      <c r="AD11">
         <v>209000</v>
       </c>
-      <c r="AD11">
+      <c r="AE11">
         <v>270000</v>
       </c>
-      <c r="AE11">
+      <c r="AF11">
         <v>183000</v>
       </c>
-      <c r="AF11">
+      <c r="AG11">
         <v>190000</v>
       </c>
-      <c r="AG11">
+      <c r="AH11">
         <v>250000</v>
       </c>
-      <c r="AH11">
+      <c r="AI11">
         <v>240000</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1108,21 +1126,24 @@
         <v>49</v>
       </c>
       <c r="W12">
+        <v>225</v>
+      </c>
+      <c r="X12">
         <v>96</v>
       </c>
-      <c r="X12">
+      <c r="Y12">
         <v>84</v>
       </c>
-      <c r="Z12">
+      <c r="AA12">
         <v>730</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Add Alex555 to spectra
</commit_message>
<xml_diff>
--- a/FluorophoreProps.xlsx
+++ b/FluorophoreProps.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
   <si>
     <t>Quantum Yield</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>mScarlet-I</t>
+  </si>
+  <si>
+    <t>AlexaFluor 555</t>
   </si>
 </sst>
 </file>
@@ -592,13 +595,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI35"/>
+  <dimension ref="A1:AJ35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="J8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="O8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="W13" sqref="W13"/>
+      <selection pane="bottomRight" activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,12 +609,12 @@
     <col min="1" max="1" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -628,7 +631,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -665,41 +668,41 @@
       <c r="U5">
         <v>7</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>58</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>1</v>
       </c>
-      <c r="Y5">
+      <c r="Z5">
         <v>7</v>
       </c>
-      <c r="AA5">
+      <c r="AB5">
         <v>7</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>59</v>
       </c>
       <c r="AD5" t="s">
         <v>59</v>
       </c>
-      <c r="AE5">
-        <v>5</v>
+      <c r="AE5" t="s">
+        <v>59</v>
       </c>
       <c r="AF5">
         <v>5</v>
       </c>
       <c r="AG5">
+        <v>5</v>
+      </c>
+      <c r="AH5">
         <v>8</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AI5" t="s">
         <v>59</v>
       </c>
-      <c r="AI5">
+      <c r="AJ5">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -764,49 +767,52 @@
         <v>41</v>
       </c>
       <c r="V7" t="s">
+        <v>66</v>
+      </c>
+      <c r="W7" t="s">
         <v>48</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>65</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Y7" t="s">
         <v>7</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="Z7" t="s">
         <v>42</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>49</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AB7" t="s">
         <v>43</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AC7" t="s">
         <v>50</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>51</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AE7" t="s">
         <v>52</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AF7" t="s">
         <v>8</v>
       </c>
-      <c r="AF7" t="s">
+      <c r="AG7" t="s">
         <v>9</v>
       </c>
-      <c r="AG7" t="s">
+      <c r="AH7" t="s">
         <v>54</v>
       </c>
-      <c r="AH7" t="s">
+      <c r="AI7" t="s">
         <v>55</v>
       </c>
-      <c r="AI7" t="s">
+      <c r="AJ7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -871,43 +877,46 @@
         <v>0.6</v>
       </c>
       <c r="V8">
+        <v>0.1</v>
+      </c>
+      <c r="W8">
         <v>0.15</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <v>0.54</v>
       </c>
-      <c r="X8">
+      <c r="Y8">
         <v>0.22</v>
       </c>
-      <c r="Y8">
+      <c r="Z8">
         <v>0.4</v>
       </c>
-      <c r="Z8">
+      <c r="AA8">
         <v>0.66</v>
       </c>
-      <c r="AA8">
+      <c r="AB8">
         <v>0.19</v>
-      </c>
-      <c r="AC8">
-        <v>0.3</v>
       </c>
       <c r="AD8">
         <v>0.3</v>
       </c>
       <c r="AE8">
+        <v>0.3</v>
+      </c>
+      <c r="AF8">
         <v>0.33</v>
       </c>
-      <c r="AF8">
+      <c r="AG8">
         <v>0.36</v>
       </c>
-      <c r="AG8">
+      <c r="AH8">
         <v>0.25</v>
       </c>
-      <c r="AI8">
+      <c r="AJ8">
         <v>0.12</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -925,20 +934,20 @@
       <c r="P9">
         <v>30</v>
       </c>
-      <c r="W9">
+      <c r="X9">
         <v>36</v>
       </c>
-      <c r="X9">
+      <c r="Y9">
         <v>15</v>
       </c>
-      <c r="Y9">
+      <c r="Z9">
         <v>20</v>
       </c>
-      <c r="AA9">
+      <c r="AB9">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -960,23 +969,26 @@
       <c r="T10">
         <v>4.0999999999999996</v>
       </c>
-      <c r="W10">
+      <c r="V10">
+        <v>0.3</v>
+      </c>
+      <c r="X10">
         <v>3.1</v>
       </c>
-      <c r="Z10">
+      <c r="AA10">
         <v>3.9</v>
       </c>
-      <c r="AB10">
+      <c r="AC10">
         <v>3.2</v>
       </c>
-      <c r="AE10">
+      <c r="AF10">
         <v>1</v>
       </c>
-      <c r="AF10">
+      <c r="AG10">
         <v>1.2</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1041,49 +1053,52 @@
         <v>58000</v>
       </c>
       <c r="V11">
+        <v>155000</v>
+      </c>
+      <c r="W11">
         <v>150000</v>
       </c>
-      <c r="W11">
+      <c r="X11">
         <v>104000</v>
       </c>
-      <c r="X11">
+      <c r="Y11">
         <v>72000</v>
       </c>
-      <c r="Y11">
+      <c r="Z11">
         <v>62500</v>
       </c>
-      <c r="Z11">
+      <c r="AA11">
         <v>92000</v>
       </c>
-      <c r="AA11">
+      <c r="AB11">
         <v>87000</v>
       </c>
-      <c r="AB11">
+      <c r="AC11">
         <v>159000</v>
       </c>
-      <c r="AC11">
+      <c r="AD11">
         <v>250000</v>
       </c>
-      <c r="AD11">
+      <c r="AE11">
         <v>209000</v>
       </c>
-      <c r="AE11">
+      <c r="AF11">
         <v>270000</v>
       </c>
-      <c r="AF11">
+      <c r="AG11">
         <v>183000</v>
       </c>
-      <c r="AG11">
+      <c r="AH11">
         <v>190000</v>
       </c>
-      <c r="AH11">
+      <c r="AI11">
         <v>250000</v>
       </c>
-      <c r="AI11">
+      <c r="AJ11">
         <v>240000</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1125,25 +1140,25 @@
       <c r="S12">
         <v>49</v>
       </c>
-      <c r="W12">
+      <c r="X12">
         <v>225</v>
       </c>
-      <c r="X12">
+      <c r="Y12">
         <v>96</v>
       </c>
-      <c r="Y12">
+      <c r="Z12">
         <v>84</v>
       </c>
-      <c r="AA12">
+      <c r="AB12">
         <v>730</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Edits for calibration of light sources
</commit_message>
<xml_diff>
--- a/FluorophoreProps.xlsx
+++ b/FluorophoreProps.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28185" windowHeight="10875"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="72">
   <si>
     <t>Quantum Yield</t>
   </si>
@@ -239,12 +239,73 @@
   <si>
     <t>AlexaFluor 555</t>
   </si>
+  <si>
+    <t>Ateam FRET pair</t>
+  </si>
+  <si>
+    <t>Ateam_donor</t>
+  </si>
+  <si>
+    <t>cp173</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tomosugi, Wataru, Tomoki Matsuda, Tomomi Tani, Tomomi Nemoto, Ippei Kotera, Kenta Saito, Kazuki Horikawa, and Takeharu Nagai. 2009. “An Ultramarine Fluorescent Protein with Increased Photostability and pH Insensitivity.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nature Methods</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 6 (5): 351–53.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Imamura, Hiromi, Kim P. Huynh Nhat, Hiroko Togawa, Kenta Saito, Ryota Iino, Yasuyuki Kato-Yamada, Takeharu Nagai, and Hiroyuki Noji. 2009. “Visualization of ATP Levels inside Single Living Cells with Fluorescence Resonance Energy Transfer-Based Genetically Encoded Indicators.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Proceedings of the National Academy of Sciences of the United States of America</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 106 (37): 15651–56.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,6 +328,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -288,9 +355,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,13 +666,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ35"/>
+  <dimension ref="A1:AL36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="O8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="V10" sqref="V10"/>
+      <selection pane="bottomRight" activeCell="A35" sqref="A35:B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,12 +680,18 @@
     <col min="1" max="1" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="2"/>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -630,8 +707,14 @@
       <c r="P4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL4" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -701,8 +784,18 @@
       <c r="AJ5">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK5" s="2">
+        <v>10</v>
+      </c>
+      <c r="AL5" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AK6" s="2"/>
+      <c r="AL6" s="2"/>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -811,8 +904,14 @@
       <c r="AJ7" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL7" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -915,8 +1014,14 @@
       <c r="AJ8">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK8" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="AL8" s="4">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -946,8 +1051,10 @@
       <c r="AB9">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK9" s="2"/>
+      <c r="AL9" s="2"/>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -987,8 +1094,10 @@
       <c r="AG10">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK10" s="2"/>
+      <c r="AL10" s="2"/>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1097,8 +1206,14 @@
       <c r="AJ11">
         <v>240000</v>
       </c>
-    </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK11" s="2">
+        <v>30000</v>
+      </c>
+      <c r="AL11" s="2">
+        <v>92000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1152,13 +1267,25 @@
       <c r="AB12">
         <v>730</v>
       </c>
-    </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK12" s="2"/>
+      <c r="AL12" s="2"/>
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AK13" s="2"/>
+      <c r="AL13" s="2"/>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AK14" s="3"/>
+      <c r="AL14" s="3"/>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK15" s="2"/>
+      <c r="AL15" s="2"/>
+    </row>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1168,13 +1295,17 @@
       <c r="H16">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="AK16" s="2"/>
+      <c r="AL16" s="2"/>
+    </row>
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="AK17" s="3"/>
+      <c r="AL17" s="3"/>
+    </row>
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1184,60 +1315,86 @@
       <c r="H18">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="AK18" s="3"/>
+      <c r="AL18" s="3"/>
+    </row>
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="AK19" s="3"/>
+      <c r="AL19" s="3"/>
+    </row>
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="AK20" s="3"/>
+      <c r="AL20" s="3"/>
+    </row>
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AK21" s="3"/>
+      <c r="AL21" s="3"/>
+    </row>
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AK22" s="3"/>
+      <c r="AL22" s="3"/>
+    </row>
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>18</v>
       </c>
       <c r="B23" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="AK23" s="3"/>
+      <c r="AL23" s="3"/>
+    </row>
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="AK24" s="3"/>
+      <c r="AL24" s="3"/>
+    </row>
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="AK25" s="3"/>
+      <c r="AL25" s="3"/>
+    </row>
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
       <c r="B26" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="AK26" s="3"/>
+      <c r="AL26" s="3"/>
+    </row>
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2</v>
       </c>
       <c r="B27" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="AK27" s="3"/>
+      <c r="AL27" s="3"/>
+    </row>
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3</v>
       </c>
       <c r="B28" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="AK28" s="3"/>
+      <c r="AL28" s="3"/>
+    </row>
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>4</v>
       </c>
@@ -1248,51 +1405,78 @@
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="AK29" s="3"/>
+      <c r="AL29" s="3"/>
+    </row>
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>5</v>
       </c>
       <c r="B30" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="AK30" s="3"/>
+      <c r="AL30" s="3"/>
+    </row>
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>6</v>
       </c>
       <c r="B31" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="AK31" s="3"/>
+      <c r="AL31" s="3"/>
+    </row>
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>7</v>
       </c>
       <c r="B32" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="AK32" s="3"/>
+      <c r="AL32" s="3"/>
+    </row>
+    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>8</v>
       </c>
       <c r="B33" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="AK33" s="3"/>
+      <c r="AL33" s="3"/>
+    </row>
+    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>9</v>
       </c>
       <c r="B34" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="AK34" s="3"/>
+      <c r="AL34" s="3"/>
+    </row>
+    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
         <v>10</v>
       </c>
+      <c r="B35" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK35" s="3"/>
+      <c r="AL35" s="3"/>
+    </row>
+    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>11</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK36" s="3"/>
+      <c r="AL36" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>